<commit_message>
Add led driver components to bom
+ a few other minor changes to bom
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\_vt\strawlab\projects\06 byo-camera beetrax\beetrax-byo-hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0152A4AA-F3BE-4062-AEDA-B8B8C71E7189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3978CD-E37E-4E27-90E1-5B93804DDBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="4200" windowWidth="25600" windowHeight="11270" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="246">
   <si>
     <t>no</t>
   </si>
@@ -466,16 +466,328 @@
   </si>
   <si>
     <t>clamping fork</t>
+  </si>
+  <si>
+    <t>MLCC 10uF 16V, size 0805</t>
+  </si>
+  <si>
+    <t>MLCC 1uF 35V, size 0805</t>
+  </si>
+  <si>
+    <t>Electrolytic capacitor 3300uF 35V</t>
+  </si>
+  <si>
+    <t>MLCC 22uF 6.5V, size 0805</t>
+  </si>
+  <si>
+    <t>MLCC 200pF 6.5V, size 0603</t>
+  </si>
+  <si>
+    <t>schottky diode (Micro-MELF)</t>
+  </si>
+  <si>
+    <t>schottky diode size 0805</t>
+  </si>
+  <si>
+    <t>0.1 inch pin header straight 1x8</t>
+  </si>
+  <si>
+    <t>SMA connector through-hole</t>
+  </si>
+  <si>
+    <t>0.1-inch socket (through-hole) 2x3</t>
+  </si>
+  <si>
+    <t>0.1-inch pin header straight 1x3</t>
+  </si>
+  <si>
+    <t>XT-30 connector</t>
+  </si>
+  <si>
+    <t>n-channel MOSFET</t>
+  </si>
+  <si>
+    <t>resistor 20 KOhm, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 510 ohm, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 10 ohms, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 0.05 ohm, size 2010</t>
+  </si>
+  <si>
+    <t>1 Ohm 1 W through-hole resistor</t>
+  </si>
+  <si>
+    <t>resistor 51 ohms, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 1 KOhm, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 10 KOhm, size 0605</t>
+  </si>
+  <si>
+    <t>resistor 4.3 KOhm, size 0605</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi Pico</t>
+  </si>
+  <si>
+    <t>gate driver UCC27624DR</t>
+  </si>
+  <si>
+    <t>LM317L (SOT-89)</t>
+  </si>
+  <si>
+    <t>7805 (TO220)</t>
+  </si>
+  <si>
+    <t>BAS85-GS08</t>
+  </si>
+  <si>
+    <t>SD0805S020S1R0</t>
+  </si>
+  <si>
+    <t>471-SMACONNECTOR</t>
+  </si>
+  <si>
+    <t>XT60U-M</t>
+  </si>
+  <si>
+    <t>TK6R7P06PL</t>
+  </si>
+  <si>
+    <t>LVK12R050DER</t>
+  </si>
+  <si>
+    <t>UCC27624DR</t>
+  </si>
+  <si>
+    <t>LM317LIPK</t>
+  </si>
+  <si>
+    <t>NJM7805FA</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>Kyocera</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>Ohmite</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>JRC</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v2</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v3</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v4</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v5</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v6</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v7</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v8</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v9</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v10</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v11</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v12</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v13</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v14</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v15</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v16</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v17</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v18</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v19</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v20</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v21</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v22</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v23</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v24</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v25</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v26</t>
+  </si>
+  <si>
+    <t>tracking/led-driver/dual-cam-pcb-v27</t>
+  </si>
+  <si>
+    <t>bypass cap, value is not critical</t>
+  </si>
+  <si>
+    <t>overkill. 1200uF should be enough.</t>
+  </si>
+  <si>
+    <t>affects stability of 7805, value is important</t>
+  </si>
+  <si>
+    <t>emi filter, value is important</t>
+  </si>
+  <si>
+    <t>there is a missing hole on the board as a polarity key. Plug the hole in the socket, and remove the corresponding pin from the plug.</t>
+  </si>
+  <si>
+    <t>optional (intended for connecting pan-tilt hobby servo motors)</t>
+  </si>
+  <si>
+    <t>name on pcb</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8,C9</t>
+  </si>
+  <si>
+    <t>D2,D1</t>
+  </si>
+  <si>
+    <t>D4,D5,D3</t>
+  </si>
+  <si>
+    <t>J2,J1</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4,J5</t>
+  </si>
+  <si>
+    <t>J6, J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R14,R16,R15,R17</t>
+  </si>
+  <si>
+    <t>R19,R6,R2,R3,R8,R13,R5,R18,R4</t>
+  </si>
+  <si>
+    <t>R20,R21</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>LPRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,13 +813,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -521,9 +841,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}" name="Table1" displayName="Table1" ref="A9:K56" totalsRowShown="0">
-  <autoFilter ref="A9:K56" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}" name="Table1" displayName="Table1" ref="A9:L82" totalsRowShown="0">
+  <autoFilter ref="A9:L82" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{9442F240-FACF-48B0-A1BF-B6F8225D9FD1}" name="no"/>
     <tableColumn id="2" xr3:uid="{22CE39F6-6E8A-482E-97B6-A27252CDE540}" name="system"/>
     <tableColumn id="3" xr3:uid="{5E4502C3-C2EC-479A-8776-C0A6BBCFDDAF}" name="type"/>
@@ -531,10 +851,11 @@
     <tableColumn id="5" xr3:uid="{6EA6D107-556D-43C7-94F3-DBF52C375317}" name="brand"/>
     <tableColumn id="6" xr3:uid="{3EDF3967-E4EC-4EA5-AB94-3E15BB3250CA}" name="part number"/>
     <tableColumn id="7" xr3:uid="{5734C5BC-8993-4775-8642-7D44F9BE9BE5}" name="count"/>
-    <tableColumn id="8" xr3:uid="{D2100962-C290-4490-BBCE-2E4CB6303B98}" name="detail"/>
+    <tableColumn id="8" xr3:uid="{D2100962-C290-4490-BBCE-2E4CB6303B98}" name="detail" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{BD03E861-E3FA-4E35-B5B9-077968FFB1E2}" name="link"/>
     <tableColumn id="10" xr3:uid="{012ADCF9-EBA3-48EA-83F6-94F95E2AA753}" name="3d model"/>
     <tableColumn id="11" xr3:uid="{3EA5F357-5442-474B-A78E-AA741C692960}" name="pcb project"/>
+    <tableColumn id="12" xr3:uid="{A63E8896-5260-4A51-87A2-C23E20CD2CB6}" name="name on pcb"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,23 +1158,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25A315E-DF31-4262-87C2-ADD015BB9516}">
-  <dimension ref="A9:K56"/>
+  <dimension ref="A9:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" customWidth="1"/>
-    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="38.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -875,7 +1197,7 @@
       <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I9" t="s">
@@ -887,19 +1209,22 @@
       <c r="K9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -918,11 +1243,11 @@
       <c r="G11">
         <v>2</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -941,11 +1266,11 @@
       <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -965,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -978,11 +1303,11 @@
       <c r="G14">
         <v>2</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1346,7 @@
       <c r="G16">
         <v>2</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1058,7 +1383,7 @@
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K18" t="s">
@@ -1084,7 +1409,7 @@
       <c r="G19">
         <v>24</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1107,7 +1432,7 @@
       <c r="G20">
         <v>24</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1124,7 +1449,7 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1144,7 +1469,7 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="J22" t="s">
@@ -1187,7 +1512,7 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1238,7 +1563,7 @@
       <c r="G27">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1255,7 +1580,7 @@
       <c r="G28">
         <v>2</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1272,7 +1597,7 @@
       <c r="G29">
         <v>2</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1329,7 +1654,7 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1349,7 +1674,7 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1369,7 +1694,7 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1403,7 +1728,7 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1440,7 +1765,7 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1480,7 +1805,7 @@
       <c r="G40">
         <v>1</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1517,7 +1842,7 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="1" t="s">
         <v>117</v>
       </c>
       <c r="J42" t="s">
@@ -1554,7 +1879,7 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="1" t="s">
         <v>118</v>
       </c>
       <c r="J44" t="s">
@@ -1617,7 +1942,7 @@
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1631,11 +1956,17 @@
       <c r="D48" t="s">
         <v>126</v>
       </c>
+      <c r="F48" t="s">
+        <v>90</v>
+      </c>
       <c r="G48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>96</v>
       </c>
@@ -1654,11 +1985,11 @@
       <c r="G49">
         <v>4</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>96</v>
       </c>
@@ -1677,11 +2008,11 @@
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>96</v>
       </c>
@@ -1700,11 +2031,11 @@
       <c r="G51">
         <v>2</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>96</v>
       </c>
@@ -1723,11 +2054,11 @@
       <c r="G52">
         <v>1</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>96</v>
       </c>
@@ -1746,11 +2077,11 @@
       <c r="G53">
         <v>1</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>96</v>
       </c>
@@ -1770,7 +2101,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
       <c r="D55" t="s">
         <v>140</v>
       </c>
@@ -1784,7 +2121,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s">
+        <v>29</v>
+      </c>
       <c r="D56" t="s">
         <v>143</v>
       </c>
@@ -1798,7 +2141,609 @@
         <v>1</v>
       </c>
     </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>144</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" t="s">
+        <v>145</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K58" t="s">
+        <v>62</v>
+      </c>
+      <c r="L58" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K59" t="s">
+        <v>62</v>
+      </c>
+      <c r="L59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K60" t="s">
+        <v>62</v>
+      </c>
+      <c r="L60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" t="s">
+        <v>148</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K61" t="s">
+        <v>62</v>
+      </c>
+      <c r="L61" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" t="s">
+        <v>179</v>
+      </c>
+      <c r="F62" t="s">
+        <v>170</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="K62" t="s">
+        <v>62</v>
+      </c>
+      <c r="L62" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" t="s">
+        <v>171</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="K63" t="s">
+        <v>62</v>
+      </c>
+      <c r="L63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="s">
+        <v>151</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="K64" t="s">
+        <v>62</v>
+      </c>
+      <c r="L64" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E65" t="s">
+        <v>245</v>
+      </c>
+      <c r="F65" t="s">
+        <v>172</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="K65" t="s">
+        <v>62</v>
+      </c>
+      <c r="L65" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>195</v>
+      </c>
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="K66" t="s">
+        <v>62</v>
+      </c>
+      <c r="L66" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>196</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K67" t="s">
+        <v>62</v>
+      </c>
+      <c r="L67" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" t="s">
+        <v>80</v>
+      </c>
+      <c r="F68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>62</v>
+      </c>
+      <c r="L68" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" t="s">
+        <v>181</v>
+      </c>
+      <c r="F69" t="s">
+        <v>174</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="K69" t="s">
+        <v>62</v>
+      </c>
+      <c r="L69" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>199</v>
+      </c>
+      <c r="C70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" t="s">
+        <v>157</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>62</v>
+      </c>
+      <c r="L70" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>200</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>158</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="K71" t="s">
+        <v>62</v>
+      </c>
+      <c r="L71" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>159</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="K72" t="s">
+        <v>62</v>
+      </c>
+      <c r="L72" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>160</v>
+      </c>
+      <c r="E73" t="s">
+        <v>182</v>
+      </c>
+      <c r="F73" t="s">
+        <v>175</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>62</v>
+      </c>
+      <c r="L73" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>203</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+      <c r="G74">
+        <v>4</v>
+      </c>
+      <c r="K74" t="s">
+        <v>62</v>
+      </c>
+      <c r="L74" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>204</v>
+      </c>
+      <c r="C75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" t="s">
+        <v>162</v>
+      </c>
+      <c r="G75">
+        <v>9</v>
+      </c>
+      <c r="K75" t="s">
+        <v>62</v>
+      </c>
+      <c r="L75" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>163</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="K76" t="s">
+        <v>62</v>
+      </c>
+      <c r="L76" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77" t="s">
+        <v>164</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="K77" t="s">
+        <v>62</v>
+      </c>
+      <c r="L77" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" t="s">
+        <v>165</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="K78" t="s">
+        <v>62</v>
+      </c>
+      <c r="L78" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>208</v>
+      </c>
+      <c r="C79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>166</v>
+      </c>
+      <c r="E79" t="s">
+        <v>183</v>
+      </c>
+      <c r="F79" t="s">
+        <v>166</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="K79" t="s">
+        <v>62</v>
+      </c>
+      <c r="L79" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" t="s">
+        <v>167</v>
+      </c>
+      <c r="E80" t="s">
+        <v>184</v>
+      </c>
+      <c r="F80" t="s">
+        <v>176</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>62</v>
+      </c>
+      <c r="L80" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>210</v>
+      </c>
+      <c r="C81" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" t="s">
+        <v>168</v>
+      </c>
+      <c r="E81" t="s">
+        <v>184</v>
+      </c>
+      <c r="F81" t="s">
+        <v>177</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="K81" t="s">
+        <v>62</v>
+      </c>
+      <c r="L81" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>211</v>
+      </c>
+      <c r="C82" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82" t="s">
+        <v>185</v>
+      </c>
+      <c r="F82" t="s">
+        <v>178</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="K82" t="s">
+        <v>62</v>
+      </c>
+      <c r="L82" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>